<commit_message>
Recent Changes by today
PrePostdeployment steps
</commit_message>
<xml_diff>
--- a/manualSteps/PrePostDeploymentSteps.xlsx
+++ b/manualSteps/PrePostDeploymentSteps.xlsx
@@ -5,10 +5,10 @@
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\css116284\Documents\backup\Salesforce\manualSteps\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\css116284\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{C16DCCDB-8B6A-41B9-A5B8-2E9EF564E3CA}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{8A36939E-1C48-4F34-9A69-51B29685A4B6}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="16575" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="68">
   <si>
     <t>Steps</t>
   </si>
@@ -156,9 +156,6 @@
     <t>Delete field "End Date" from Course Object</t>
   </si>
   <si>
-    <t>Delete field "Post Code" from Booking Object</t>
-  </si>
-  <si>
     <t>Delete field "Start Date" from Course Object</t>
   </si>
   <si>
@@ -222,64 +219,25 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">
-Goto -&gt; Setup -&gt; Create -&gt; Objects 
-Click Booking 
-Goto Section "Custom Fields &amp; Relationships"
-Click Del against field lavel "PostCode"
-Select Checkbox against "Yes, I want to delete the custom formula"
-Click Delete
-</t>
-  </si>
-  <si>
     <t>Reference</t>
   </si>
   <si>
     <t>Community license for Profiles</t>
   </si>
   <si>
-    <t xml:space="preserve">Go to setup--&gt;Quick Find--&gt;Communities --&gt;All Communities --&gt;Go to Workspaces next to community
-Go to Administration (wrench Icon symbol) Template--&gt;Go to Members list--&gt;Add select Profiles--&gt;Membership co-ordinator--&gt; save
-</t>
-  </si>
-  <si>
     <t>OWD &amp; Sharing rules creation</t>
   </si>
   <si>
     <t>Sharing Sets</t>
   </si>
   <si>
-    <t>Go to setup --&gt;Quick Find--&gt;Communities Settings--&gt;select Sharing sets--&gt;Click New, Give  "Parent Access" as label name --&gt;Sharing set name "Parent_Access"--&gt;Then Select profile "Customer Community Login User" and "Membership coordinator"--&gt;Select objects "Case"
- Go to Configure Access label- click on setup--&gt;  user:account--&gt; select Target :Case-Contact.Account--&gt;Access Level-Read/write--save</t>
-  </si>
-  <si>
     <t>Profile Permissions(FLS, CRUD)</t>
   </si>
   <si>
-    <t xml:space="preserve">Go to setup --&gt;In Administer, Go to Profiles --&gt; select "Membership coordinator"--&gt;Field-Level Security--&gt;select Custom Field-Level Security Or Standard Field-Level Security --&gt; Provide Basic Access &amp; Data Administration if required--click on "Recurring Donations"[View]--&gt;click on Edit--&gt;select read access Check box--&gt;select Edit Access check box--&gt;save
-</t>
-  </si>
-  <si>
     <t>Queue</t>
   </si>
   <si>
-    <t xml:space="preserve">Go to setup--&gt;Quick Find--&gt;Queues--&gt;click on New--&gt;Label:  Enquiries Team  --&gt;Queue Name 
-: Enquiries Team  --&gt;Queue Email:"swathi.kota@csscorp.com"  --&gt;Supported Objects:Case  --&gt;Queue Members--&gt;" Users"--&gt;click on Save.
-Remaining Queue Names: Course_Booking_Queue, Branch_Queue,Booking_Enquiry
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Go to setup--&gt;Quick Find--&gt;Queues--&gt;click on New--&gt;Label:  Finance --&gt;Queue Name 
-: Finance  --&gt;Queue Email:"Mahanth Garlapati"  --&gt;Supported Objects:Payment Schedule --&gt;Queue Members--&gt;" Mahanth Garlapati"--&gt;click on Save.
-</t>
-  </si>
-  <si>
     <t>Public group</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Go to setup--&gt;Quick Find--&gt;Public Groups--&gt;click on New--&gt;Add Label Name:Enquiry Psa Group --&gt;Add Users:Enquires Team--&gt;Click Save
-Remaining Public Groups:Branch co-ordinator group,Capacity PSA Group,ProjectLego Group,Request to be a volunteer,Volunteer Group,Yoga Co-Ordinator Course drop in Users
-</t>
   </si>
   <si>
     <t xml:space="preserve">Classic </t>
@@ -390,19 +348,6 @@
     <t>Publish Sites for Community "NCTParentCustomer"</t>
   </si>
   <si>
-    <t xml:space="preserve">Go to setup--&gt;In Administer, click on sharing settings--&gt;click New button of specific object --&gt;Account Sharing Rules--&gt;New--&gt; Label:Read/Write access  --&gt;
-Rule Name : Read_Write_access --&gt; 
-Based on criteria: Owner in Group: Branch co-ordinator group--&gt;
-owned by members of Group: Branch co-ordinator group--&gt;
-Share with Group: Branch co-ordinator group--&gt;
-Default Account, Contract and Asset Access:Read/Write--&gt;
-Contact Access:Read/Write--&gt;
-Opportunity Access:Read/Write--&gt;
-Case Access:Read/Write--&gt;
-Click Save "Button"
-</t>
-  </si>
-  <si>
     <r>
       <rPr>
         <b/>
@@ -435,14 +380,165 @@
 </t>
     </r>
   </si>
+  <si>
+    <t>Go to setup 
+Quick Find
+Communities Settings
+select Sharing sets
+Click New, Give  "Parent Access" as label name 
+Sharing set name "Parent_Access"
+Then Select profile "Customer Community Login User" and "Membership coordinator"
+Select objects "Case"
+Go to Configure Access label- click on setup
+User:account
+Select Target :Case Contact.Account
+Access Level-Read/write
+Click on save Button</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Go to setup
+Click on sharing settings
+Click New button of specific object 
+Go to Account Sharing Rules
+Select New Button
+Label:Read/Write access  
+Rule Name : Read_Write_access
+Based on criteria: Owner in Group: Branch co-ordinator group
+owned by members of Group: Branch co-ordinator group
+Share with Group: Branch co-ordinator group
+Default Account, Contract and Asset Access:Read/Write
+Contact Access:Read/Write
+Opportunity Access:Read/Write
+Case Access:Read/Write
+Click Save "Button"
+</t>
+  </si>
+  <si>
+    <t>Go to setup 
+Quick Find
+In Administer, Go to Profiles 
+Select "Membership coordinator"
+Select Field-Level Security
+Select Custom Field-Level Security Or Standard Field-Level Security 
+Provide Basic Access &amp; Data Administration if required
+Click on "Recurring Donations"[View]
+Click on Edit
+Select read access Check box
+Select Edit Access check box
+Click save Button.</t>
+  </si>
+  <si>
+    <t>Go to setup
+Quick Find
+SelectCommunities 
+Selectelect All Communities 
+Go to Workspaces next to community
+Go to Administration (wrench Icon symbol) Template
+Go to Members listAdd select Profiles
+Membership co-ordinator
+Click on save</t>
+  </si>
+  <si>
+    <t>Go to setup
+Quick Find
+Queues
+click on New Button 
+Label:  Enquiries Team  
+Queue Name : Enquiries Team  
+Queue Email:"swathi.kota@csscorp.com"  
+Supported Objects:Case  
+Queue Members: " Users"
+Click on Save.
+Remaining Queue Names: Course_Booking_Queue, Branch_Queue,Booking_Enquiry</t>
+  </si>
+  <si>
+    <t>Go to setup
+Quick Find
+Queues
+Click on New Button
+Label:  Finance 
+Queue Name : Finance  
+Queue Email:"Mahanth Garlapati"  
+Supported Objects:Payment Schedule 
+Queue Members: " Mahanth Garlapati"
+Click on Save.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Go to setup
+Quick Find
+Public Groups
+click on New
+Add Label Name:Enquiry Psa Group 
+Add Users:Enquires Team
+Click Save button
+Remaining Public Groups:Branch co-ordinator group,Capacity PSA Group,ProjectLego Group,Request to be a volunteer,Volunteer Group,Yoga Co-Ordinator Course drop in Users
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Create Site "PaymentLink" Goto -&gt; Setup -&gt; Develop -&gt; Lightning Components -&gt; Sites
+Click New
+Fill the following fields with below values.
+  1. Site Label : PaymentLink
+  2. Site Name: PaymentLink
+  3. Site Contact: Current_User (This needs to be updated in future)
+  4. Default Web Address: "PaymentLinkProcessor"
+  5. Active: Select the checkbox
+  6. Active Site Home Page: PaymentLinkProcessor
+and leave rest of the fields to the default.
+Click Save.
+</t>
+  </si>
+  <si>
+    <t>Create Site "PaymentLink"</t>
+  </si>
+  <si>
+    <t>Lightning</t>
+  </si>
+  <si>
+    <t>Update Site URL values for Stripe Payment
+ in Payment Hub.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Goto Select App Launcher  
+Click on "StepOrange CPM" 
+From TabMenu 
+Click on Setup
+Goto Section "Extensions PSP"  
+Click "PaymentHub-Stripe"
+Remove the production url value from "Push URL" field.
+Goto  Setup 
+Quick Find
+Select  Sites 
+Copy the "Site URL" value for Site "CreditCardPayment".
+Now paste that value in the "Push URL" field on "PaymentHub-Stripe".
+Once done the "Webhook URL" field also automatically gets updated with the latest url pasted just now.
+Remove the value for field "Publishable Key(Production)".
+Update the value for filed "Publishable Key(Test)" with the value that is in PreUAT. 
+Also Enable the slidebar for field "IsTest".
+</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -566,29 +662,29 @@
   </borders>
   <cellStyleXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
@@ -606,7 +702,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -627,28 +723,40 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="13" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="13" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="13" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="13" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="13" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="13" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="13" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="13" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="13" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="13" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="13" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="13" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="13" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="13" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1052,10 +1160,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L52"/>
+  <dimension ref="A1:L51"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1070,17 +1178,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A1" s="22"/>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22"/>
-      <c r="G1" s="22"/>
-      <c r="H1" s="22"/>
-      <c r="I1" s="22"/>
-      <c r="J1" s="22"/>
-      <c r="K1" s="22"/>
+      <c r="A1" s="27"/>
+      <c r="B1" s="27"/>
+      <c r="C1" s="27"/>
+      <c r="D1" s="27"/>
+      <c r="E1" s="27"/>
+      <c r="F1" s="27"/>
+      <c r="G1" s="27"/>
+      <c r="H1" s="27"/>
+      <c r="I1" s="27"/>
+      <c r="J1" s="27"/>
+      <c r="K1" s="27"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -1117,7 +1225,7 @@
         <v>8</v>
       </c>
       <c r="L2" s="3" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="3" spans="1:12" ht="221.25" thickBot="1" x14ac:dyDescent="0.3">
@@ -1278,7 +1386,7 @@
         <v>27</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E10" s="8"/>
       <c r="F10" s="8"/>
@@ -1296,10 +1404,10 @@
         <v>12</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E11" s="8"/>
       <c r="F11" s="8"/>
@@ -1317,10 +1425,10 @@
         <v>12</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E12" s="8"/>
       <c r="F12" s="8"/>
@@ -1341,7 +1449,7 @@
         <v>30</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E13" s="8"/>
       <c r="F13" s="8"/>
@@ -1362,7 +1470,7 @@
         <v>31</v>
       </c>
       <c r="D14" s="8" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E14" s="8"/>
       <c r="F14" s="8"/>
@@ -1372,18 +1480,18 @@
       <c r="J14" s="8"/>
       <c r="K14" s="8"/>
     </row>
-    <row r="15" spans="1:12" ht="127.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:12" ht="96" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="7">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B15" s="7" t="s">
         <v>12</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>32</v>
+        <v>54</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>34</v>
+        <v>53</v>
       </c>
       <c r="E15" s="8"/>
       <c r="F15" s="8"/>
@@ -1393,40 +1501,19 @@
       <c r="J15" s="8"/>
       <c r="K15" s="8"/>
     </row>
-    <row r="16" spans="1:12" ht="96" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="7">
-        <v>14</v>
-      </c>
-      <c r="B16" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="C16" s="8" t="s">
-        <v>62</v>
-      </c>
-      <c r="D16" s="8" t="s">
-        <v>61</v>
-      </c>
-      <c r="E16" s="8"/>
-      <c r="F16" s="8"/>
-      <c r="G16" s="8"/>
-      <c r="H16" s="8"/>
-      <c r="I16" s="8"/>
-      <c r="J16" s="8"/>
-      <c r="K16" s="8"/>
-    </row>
-    <row r="17" ht="16.5" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="51" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="6"/>
-      <c r="B51" s="6"/>
-      <c r="C51" s="6"/>
-      <c r="D51" s="6"/>
-      <c r="E51" s="6"/>
-      <c r="F51" s="6"/>
-      <c r="G51" s="6"/>
-      <c r="H51" s="6"/>
-      <c r="I51" s="6"/>
-    </row>
-    <row r="52" spans="1:9" ht="16.5" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="16" spans="1:12" ht="16.5" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="50" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A50" s="6"/>
+      <c r="B50" s="6"/>
+      <c r="C50" s="6"/>
+      <c r="D50" s="6"/>
+      <c r="E50" s="6"/>
+      <c r="F50" s="6"/>
+      <c r="G50" s="6"/>
+      <c r="H50" s="6"/>
+      <c r="I50" s="6"/>
+    </row>
+    <row r="51" spans="1:9" ht="16.5" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:K1"/>
@@ -1445,8 +1532,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A08E240A-CAE5-4B6F-872D-9A32F7494C09}">
   <dimension ref="A2:K11"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1492,7 +1579,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="180" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" ht="213" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -1500,10 +1587,10 @@
         <v>12</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D3" s="11" t="s">
-        <v>41</v>
+        <v>59</v>
       </c>
       <c r="E3" s="10"/>
       <c r="F3" s="10"/>
@@ -1513,7 +1600,7 @@
       <c r="J3" s="10"/>
       <c r="K3" s="10"/>
     </row>
-    <row r="4" spans="1:11" ht="207.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" ht="334.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="12">
         <v>2</v>
       </c>
@@ -1521,10 +1608,10 @@
         <v>12</v>
       </c>
       <c r="C4" s="13" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="E4" s="13"/>
       <c r="F4" s="13"/>
@@ -1534,7 +1621,7 @@
       <c r="J4" s="13"/>
       <c r="K4" s="13"/>
     </row>
-    <row r="5" spans="1:11" ht="152.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" ht="213.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="14">
         <v>3</v>
       </c>
@@ -1542,10 +1629,10 @@
         <v>12</v>
       </c>
       <c r="C5" s="15" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>44</v>
+        <v>56</v>
       </c>
       <c r="E5" s="15"/>
       <c r="F5" s="15"/>
@@ -1555,7 +1642,7 @@
       <c r="J5" s="15"/>
       <c r="K5" s="15"/>
     </row>
-    <row r="6" spans="1:11" ht="227.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" ht="255.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="14">
         <v>4</v>
       </c>
@@ -1563,10 +1650,10 @@
         <v>12</v>
       </c>
       <c r="C6" s="15" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>46</v>
+        <v>58</v>
       </c>
       <c r="E6" s="15"/>
       <c r="F6" s="15"/>
@@ -1576,7 +1663,7 @@
       <c r="J6" s="15"/>
       <c r="K6" s="15"/>
     </row>
-    <row r="7" spans="1:11" ht="153.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" ht="208.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="14">
         <v>5</v>
       </c>
@@ -1584,10 +1671,10 @@
         <v>12</v>
       </c>
       <c r="C7" s="15" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>48</v>
+        <v>60</v>
       </c>
       <c r="E7" s="15"/>
       <c r="F7" s="15"/>
@@ -1597,7 +1684,7 @@
       <c r="J7" s="15"/>
       <c r="K7" s="15"/>
     </row>
-    <row r="8" spans="1:11" ht="148.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" ht="195.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="14">
         <v>6</v>
       </c>
@@ -1605,10 +1692,10 @@
         <v>12</v>
       </c>
       <c r="C8" s="15" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>49</v>
+        <v>61</v>
       </c>
       <c r="E8" s="15"/>
       <c r="F8" s="15"/>
@@ -1618,7 +1705,7 @@
       <c r="J8" s="15"/>
       <c r="K8" s="15"/>
     </row>
-    <row r="9" spans="1:11" ht="93.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" ht="188.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="14">
         <v>7</v>
       </c>
@@ -1626,10 +1713,10 @@
         <v>12</v>
       </c>
       <c r="C9" s="15" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>51</v>
+        <v>62</v>
       </c>
       <c r="E9" s="15"/>
       <c r="F9" s="15"/>
@@ -1639,11 +1726,19 @@
       <c r="J9" s="15"/>
       <c r="K9" s="15"/>
     </row>
-    <row r="10" spans="1:11" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="14"/>
-      <c r="B10" s="14"/>
-      <c r="C10" s="15"/>
-      <c r="D10" s="15"/>
+    <row r="10" spans="1:11" ht="190.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="14">
+        <v>8</v>
+      </c>
+      <c r="B10" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="C10" s="15" t="s">
+        <v>64</v>
+      </c>
+      <c r="D10" s="8" t="s">
+        <v>63</v>
+      </c>
       <c r="E10" s="15"/>
       <c r="F10" s="15"/>
       <c r="G10" s="15"/>
@@ -1652,7 +1747,20 @@
       <c r="J10" s="15"/>
       <c r="K10" s="15"/>
     </row>
-    <row r="11" spans="1:11" ht="16.5" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="11" spans="1:11" ht="284.25" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="25">
+        <v>9</v>
+      </c>
+      <c r="B11" s="25" t="s">
+        <v>65</v>
+      </c>
+      <c r="C11" s="26" t="s">
+        <v>66</v>
+      </c>
+      <c r="D11" s="24" t="s">
+        <v>67</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1662,8 +1770,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{45C76CEF-C2B4-465C-9D00-2F21483FAE24}">
   <dimension ref="A1:K6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1715,13 +1823,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="17" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="C2" s="18" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="D2" s="16" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="E2" s="18"/>
       <c r="F2" s="18"/>
@@ -1739,10 +1847,10 @@
         <v>12</v>
       </c>
       <c r="C3" s="18" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="D3" s="16" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="E3" s="20"/>
       <c r="F3" s="20"/>
@@ -1760,10 +1868,10 @@
         <v>12</v>
       </c>
       <c r="C4" s="21" t="s">
-        <v>57</v>
-      </c>
-      <c r="D4" s="16" t="s">
-        <v>58</v>
+        <v>49</v>
+      </c>
+      <c r="D4" s="23" t="s">
+        <v>50</v>
       </c>
       <c r="E4" s="20"/>
       <c r="F4" s="20"/>
@@ -1781,10 +1889,10 @@
         <v>12</v>
       </c>
       <c r="C5" s="21" t="s">
-        <v>59</v>
-      </c>
-      <c r="D5" s="23" t="s">
-        <v>64</v>
+        <v>51</v>
+      </c>
+      <c r="D5" s="22" t="s">
+        <v>55</v>
       </c>
       <c r="E5" s="20"/>
       <c r="F5" s="20"/>
@@ -1805,7 +1913,7 @@
         <v>25</v>
       </c>
       <c r="D6" s="16" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="E6" s="20"/>
       <c r="F6" s="20"/>

</xml_diff>

<commit_message>
Latest Changes on Profiles Queues Objects
Latest Changes on Profiles Queues Objects
</commit_message>
<xml_diff>
--- a/manualSteps/PrePostDeploymentSteps.xlsx
+++ b/manualSteps/PrePostDeploymentSteps.xlsx
@@ -5,12 +5,12 @@
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\css116284\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\css116762\Desktop\CICD\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{8A36939E-1C48-4F34-9A69-51B29685A4B6}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{59FECC70-376B-4E09-A134-9F883D82AAF5}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="16575" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="16575" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PreDeploymentSteps" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="101">
   <si>
     <t>Steps</t>
   </si>
@@ -176,36 +176,6 @@
 Click Edit against "Client" Record Type
 Change Record Type Label to "Parent"
 Click Save
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
-Goto -&gt; Setup -&gt; Create -&gt; Objects 
-Click Sessions 
-Goto Section "Custom Fields &amp; Relationships"
-Click Del against field lavel "Venue"
-Select Checkbox against "Yes, I want to delete the custom formula"
-Click Delete
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
-Goto -&gt; Setup -&gt; Create -&gt; Objects 
-Click Courses 
-Goto Section "Custom Fields &amp; Relationships"
-Click Del against field lavel "Venue"
-Select Checkbox against "Yes, I want to delete the custom formula"
-Click Delete
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
-Goto -&gt; Setup -&gt; Create -&gt; Objects 
-Click Courses 
-Goto Section "Custom Fields &amp; Relationships"
-Click Del against field lavel "Start Date"
-Select Checkbox against "Yes, I want to delete the custom formula"
-Click Delete
 </t>
   </si>
   <si>
@@ -334,14 +304,6 @@
 Click "Users"
 Click on "New User"
 Fill the "Mandary data" &amp; enable checkbox "Generate new password and notify user immediately" to save the record.
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Goto -&gt; Setup -&gt; Build -&gt; Customize -&gt; Communities -&gt; All Communities
-Click Builder for Community "NCTParentCustomer"
-Click Publish which is on top right corner of the page.
-Click Publish again on the pop up window.
-Click Got it on the pop up window.
 </t>
   </si>
   <si>
@@ -495,10 +457,6 @@
     <t>Lightning</t>
   </si>
   <si>
-    <t>Update Site URL values for Stripe Payment
- in Payment Hub.</t>
-  </si>
-  <si>
     <t xml:space="preserve">Goto Select App Launcher  
 Click on "StepOrange CPM" 
 From TabMenu 
@@ -517,14 +475,395 @@
 Also Enable the slidebar for field "IsTest".
 </t>
   </si>
+  <si>
+    <t>Update Site URL values for Stripe Payment in Payment Hub.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Create Membership Collections Target in 
+PaymentHub
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Create Course Fee Collections Target in 
+PaymentHub
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Create Training Fee Collections Target in 
+PaymentHub
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Goto AppLauncher 
+StepOrange CPM 
+Tab Menu 
+choose Setup 
+Goto  Section "Extensions-System" 
+ProcessingHub
+If Payment Processing Authentication details are provided in the below fields( if not present contact StepOrange)
+Then you will be able to see "Targets" tab.
+Click "Targets" Tab
+Click "Add Target" Button
+Fill the fileds with below information:
+1. Name : NCT Training Fee Collections - S18
+2. Target: PaymentHub BACS
+3. Type: Manual
+Click Save. 
+Now click the down arrow beside the created target click settings.
+Fill the fields with below information:
+1: Bank account addition: 30-00-09
+2. Bank account number: 02080596
+3. Collection file lead time (days) : 3
+4. Company name: NCT
+5. Company Service User Number: 836903
+6. DDI lead time: 10
+7. Number of generated files: 1
+Click Save
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Goto  AppLauncher 
+StepOrange CPM 
+Tab Menu 
+choose Setup 
+Goto  Section "Extensions-System" 
+ProcessingHub
+If Payment Processing Authentication details are provided in the below fields( if not present contact StepOrange)
+Then you will be able to see "Targets" tab.
+Click "Targets" Tab
+Click "Add Target" Button
+Fill the fileds with below information:
+1. Name : NCT Training Fee Collections - S18
+2. Target: PaymentHub BACS
+3. Type: Manual
+Click Save. 
+Now click the down arrow beside the created target click settings.
+Fill the fields with below information:
+1: Bank account addition: 30-00-09
+2. Bank account number: 02080596
+3. Collection file lead time (days) : 3
+4. Company name: NCT
+5. Company Service User Number: 836903
+6. DDI lead time: 10
+7. Number of generated files: 1
+Click Save
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Goto  AppLauncher 
+StepOrange CPM 
+Tab Menu 
+choose Setup 
+Goto  Section "Extensions-System" 
+ProcessingHub
+If Payment Processing Authentication details are provided in the below fields( if not present contact StepOrange)
+Then you will be able to see "Targets" tab.
+Click "Targets" Tab
+Click "Add Target" Button
+Fill the fileds with below information:
+1. Name : NCT Course Fee Collections - S18
+2. Target: PaymentHub BACS
+3. Type: Manual
+Click Save. 
+Now click the down arrow beside the created target click settings.
+Fill the fields with below information:
+1: Bank account addition: 30-00-09
+2. Bank account number: 07809225
+3. Collection file lead time (days) : 2
+4. Company name: NCT
+5. Company Service User Number: 836903
+6. DDI lead time: 10
+7. Number of generated files: 1
+Click Save
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Goto  AppLauncher 
+StepOrange CPM  Tab Menu
+Choose Setup 
+Goto  Section "Extensions-System"  ProcessingHub
+If Payment Processing Authentication details are provided in the below fields( if not present contact StepOrange)
+Then you will be able to see "Targets" tab.
+Click "Targets" Tab
+Click "Add Target" Button
+Fill the fileds with below information:
+1. Name : NCT Membership Collections - S18
+2. Target: PaymentHub BACS
+3. Type: Manual
+Click Save. 
+Now click the down arrow beside the created target click settings.
+Fill the fields with below information:
+1: Bank account addition: 30-00-09
+2. Bank account number: 02080596
+3. Collection file lead time (days) : 3
+4. Company name: NCT
+5. Company Service User Number: 770552
+6. DDI lead time: 10
+7. Number of generated files: 1
+Click Save
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Goto Setup
+Build 
+Customize 
+Communities  All Communities
+Click Builder for Community "NCTParentCustomer"
+Click Publish which is on top right corner of the page.
+Click Publish again on the pop up window.
+Click Got it on the pop up window.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Goto  Setup 
+Create Go to  Objects 
+Click Sessions 
+Goto Section "Custom Fields &amp; Relationships"
+Click Del against field lavel "Venue"
+Select Checkbox against "Yes, I want to delete the custom formula"
+Click Delete
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Goto  Setup 
+Create  Objects 
+Click Courses 
+Goto Section "Custom Fields &amp; Relationships"
+Click Del against field lavel "Venue"
+Select Checkbox against "Yes, I want to delete the custom formula"
+Click Delete
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Goto  Setup 
+Create Go  to  Objects 
+Click Courses 
+Goto Section "Custom Fields &amp; Relationships"
+Click Del against field lavel "Start Date"
+Select Checkbox against "Yes, I want to delete the custom formula"
+Click Delete
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Goto  Setup 
+QuickFind  Communities 
+Community Settings
+Select the Checkbox filed Enable Communities 
+In the Domain Name field add value "ournct".
+Click Save.
+</t>
+  </si>
+  <si>
+    <t>Creating a Connected App 
+"PaymentConnectedApp"</t>
+  </si>
+  <si>
+    <t>Goto -&gt; Setup -&gt; Build -&gt; Create -&gt; Click Apps
+Goto Section Connected Apps
+Click New
+Fill the fields with the below information:
+In Section: Basic Information
+1. Connected App Name: PaymentConnectedApp
+2. API Name: PaymentConnectedApp
+3. Contact Email:  users email address who is creating this connected app.
+In Section: Api (Enable OAuth Settings)
+1. Enable OAuth Settings: Select the checkbox
+2. Callback URL: https://localhost.com
+3. Selected OAuth Scopes: Full Access (full)
+4. Require Secret for Web Server Flow: Select the Checkbox
+Click Save</t>
+  </si>
+  <si>
+    <t>Login page enable</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Go to setup 
+Quick Find
+Click on All Communities  
+Click on Workspaces 
+Select Administration
+Go to Login&amp;Registration
+go to  Registration Page Configuration
+Enable the check box  Allow external users to self-register
+Registration Page Type: Visualforce Page : ParentCommunitySelfReg
+Profile: Membership coordinator
+select Account
+Click on save
+</t>
+  </si>
+  <si>
+    <t>Signup Page added</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Go to setup 
+Quick Find
+Click on All Communities  
+Click on Workspaces 
+Select Administration
+Go to Pages
+Go to Force.Com
+Click on Edit
+Click on Self Registration Page and add ParentCommunitySelfReg
+Click on Save
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Go to setup
+Object Manager
+Enter in Quick Find "Transaction"
+go to Fields &amp; Relationships click on New Button
+Check button Picklist Button
+Field Label:Data Source
+Field Name: Data_Source
+select Radio button:Enter values, with each value separated by a new line
+Add these values: Salesforce,CARE,Intrabiz
+Click on checkbox :Use first value as default value
+click next
+select Visible check box and select next button
+Click checkbox :  Transaction Layout
+Click Save button
+</t>
+  </si>
+  <si>
+    <t>Added Data source field for Transaction object</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Go to setup
+Object Manager
+Enter in Quick Find "Transaction" API Name " cpm__Transaction__c"
+go to Fields &amp; Relationships click on New Button
+Check button Picklist Button
+Field Label:Data Source
+Field Name: Data_Source
+select Radio button:Enter values, with each value separated by a new line
+Add these values: Salesforce,CARE,Intrabiz
+Click on checkbox :Use first value as default value
+click next
+select Visible check box and select next button
+Click checkbox :  Transaction Layout
+Click Save button
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Go to setup
+Quick find
+go to All Communities
+click on Builder option
+select Component option
+go to Visualforce option
+Drag in to Content section
+Give the ParentCommunityHome Page in Visualforce Page Name
+Then click on Publish option
+</t>
+  </si>
+  <si>
+    <t>Add visualforce Home page into builder</t>
+  </si>
+  <si>
+    <t>Add Logo for signup Page</t>
+  </si>
+  <si>
+    <t>Go to setup 
+Quick Find
+Click on All Communities  
+Click on Workspaces 
+Select Administration
+Go to Login&amp;Registration
+go to Branding Options 
+Logo file : Choose file from local system
+Click on Save button</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Add visualforce page into HELP tab </t>
+  </si>
+  <si>
+    <t>Go to setup
+Quick find
+go to All Communities
+click on Builder option
+select Navigation Menu
+Click on Edit Default Navigation
+Click on Add Menu Item
+give Name: Help
+Type:CommunityPage
+Page:NCTHelpTicket
+click on check box Publicly available
+Click on save button
+Then click on Publish button</t>
+  </si>
+  <si>
+    <t>Add Branding for signup Page</t>
+  </si>
+  <si>
+    <t>Go to setup 
+Quick Find
+Click on All Communities  
+Click on Workspaces 
+Select Administration
+Go to Login&amp;Registration
+go to Branding Options 
+select Branding options
+Give  Background #FFFFFF
+Login Button: #1797C0
+Click save button.</t>
+  </si>
+  <si>
+    <t>Added Data source field for
+ cpm__Transaction__c object</t>
+  </si>
+  <si>
+    <t>Publish Sites for Paymenthub</t>
+  </si>
+  <si>
+    <t>Goto -&gt; Setup -&gt; User Interface -&gt; Sites and Domains -&gt; Sites
+Click on "New" button
+Enter "Payment" value in 'Site Label'
+Enter "Payment" value in 'Site Name'
+Select "Active Site Home Page" with "nctMembershipPaymentPage"
+Click on 'Save' button.</t>
+  </si>
+  <si>
+    <t>Add "Visualforce" page in "Payment" Site which created in 15th Step.</t>
+  </si>
+  <si>
+    <t>Goto -&gt; Setup -&gt; User Interface -&gt; Sites and Domains -&gt; Sites
+Click on "Edit" button under "Site Visualforce Page"
+Add "Visualforce Page" -&gt; nctETMembershipPaymentPage, nctMembershipPayementPage, nctPaymentHubErrorMsgPage, nctPaymentHubPage, nctPaymentHubSuccessMsgPage.
+Click on "Save" button.</t>
+  </si>
+  <si>
+    <t>Add "Cutom Label" for the Payment Success and Failure Pages</t>
+  </si>
+  <si>
+    <t>Goto -&gt; Setup -&gt; User Interface -&gt; Custom Labels
+Click on "New" button.
+Enter "PAYMENTSTATUSURL" value under "Short Description" field
+Enter "PAYMENTSTATUSURL" value under "Name" field
+Enter "Payment link Site which we did in Step-15" value under "value" field.
+Click on "Save" button.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -662,29 +1001,29 @@
   </borders>
   <cellStyleXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
@@ -702,7 +1041,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -723,30 +1062,30 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="13" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="13" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="13" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="13" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="13" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="13" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="13" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="13" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="13" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="13" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="13" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="13" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="13" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="13" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -754,6 +1093,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="13" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1160,10 +1502,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L51"/>
+  <dimension ref="A1:L56"/>
   <sheetViews>
-    <sheetView topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
+      <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1178,17 +1520,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A1" s="27"/>
-      <c r="B1" s="27"/>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
-      <c r="E1" s="27"/>
-      <c r="F1" s="27"/>
-      <c r="G1" s="27"/>
-      <c r="H1" s="27"/>
-      <c r="I1" s="27"/>
-      <c r="J1" s="27"/>
-      <c r="K1" s="27"/>
+      <c r="A1" s="28"/>
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
+      <c r="F1" s="28"/>
+      <c r="G1" s="28"/>
+      <c r="H1" s="28"/>
+      <c r="I1" s="28"/>
+      <c r="J1" s="28"/>
+      <c r="K1" s="28"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -1225,7 +1567,7 @@
         <v>8</v>
       </c>
       <c r="L2" s="3" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="3" spans="1:12" ht="221.25" thickBot="1" x14ac:dyDescent="0.3">
@@ -1407,7 +1749,7 @@
         <v>28</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="E11" s="8"/>
       <c r="F11" s="8"/>
@@ -1417,7 +1759,7 @@
       <c r="J11" s="8"/>
       <c r="K11" s="8"/>
     </row>
-    <row r="12" spans="1:12" ht="127.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:12" ht="143.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="7">
         <v>10</v>
       </c>
@@ -1428,7 +1770,7 @@
         <v>29</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>35</v>
+        <v>74</v>
       </c>
       <c r="E12" s="8"/>
       <c r="F12" s="8"/>
@@ -1438,7 +1780,7 @@
       <c r="J12" s="8"/>
       <c r="K12" s="8"/>
     </row>
-    <row r="13" spans="1:12" ht="127.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:12" ht="143.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="7">
         <v>11</v>
       </c>
@@ -1449,7 +1791,7 @@
         <v>30</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>34</v>
+        <v>73</v>
       </c>
       <c r="E13" s="8"/>
       <c r="F13" s="8"/>
@@ -1459,7 +1801,7 @@
       <c r="J13" s="8"/>
       <c r="K13" s="8"/>
     </row>
-    <row r="14" spans="1:12" ht="127.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:12" ht="143.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="7">
         <v>12</v>
       </c>
@@ -1470,7 +1812,7 @@
         <v>31</v>
       </c>
       <c r="D14" s="8" t="s">
-        <v>33</v>
+        <v>72</v>
       </c>
       <c r="E14" s="8"/>
       <c r="F14" s="8"/>
@@ -1480,18 +1822,18 @@
       <c r="J14" s="8"/>
       <c r="K14" s="8"/>
     </row>
-    <row r="15" spans="1:12" ht="96" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:12" ht="143.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="7">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B15" s="7" t="s">
         <v>12</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>53</v>
+        <v>71</v>
       </c>
       <c r="E15" s="8"/>
       <c r="F15" s="8"/>
@@ -1501,19 +1843,229 @@
       <c r="J15" s="8"/>
       <c r="K15" s="8"/>
     </row>
-    <row r="16" spans="1:12" ht="16.5" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="50" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="6"/>
-      <c r="B50" s="6"/>
-      <c r="C50" s="6"/>
-      <c r="D50" s="6"/>
-      <c r="E50" s="6"/>
-      <c r="F50" s="6"/>
-      <c r="G50" s="6"/>
-      <c r="H50" s="6"/>
-      <c r="I50" s="6"/>
-    </row>
-    <row r="51" spans="1:9" ht="16.5" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="16" spans="1:12" ht="409.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="7">
+        <v>14</v>
+      </c>
+      <c r="B16" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="C16" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="D16" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="E16" s="8"/>
+      <c r="F16" s="8"/>
+      <c r="G16" s="8"/>
+      <c r="H16" s="8"/>
+      <c r="I16" s="8"/>
+      <c r="J16" s="8"/>
+      <c r="K16" s="8"/>
+    </row>
+    <row r="17" spans="1:11" ht="409.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="7">
+        <v>15</v>
+      </c>
+      <c r="B17" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="C17" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="D17" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="E17" s="8"/>
+      <c r="F17" s="8"/>
+      <c r="G17" s="8"/>
+      <c r="H17" s="8"/>
+      <c r="I17" s="8"/>
+      <c r="J17" s="8"/>
+      <c r="K17" s="8"/>
+    </row>
+    <row r="18" spans="1:11" ht="409.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="7">
+        <v>16</v>
+      </c>
+      <c r="B18" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="C18" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="D18" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="E18" s="8"/>
+      <c r="F18" s="8"/>
+      <c r="G18" s="8"/>
+      <c r="H18" s="8"/>
+      <c r="I18" s="8"/>
+      <c r="J18" s="8"/>
+      <c r="K18" s="8"/>
+    </row>
+    <row r="19" spans="1:11" ht="409.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="7">
+        <v>17</v>
+      </c>
+      <c r="B19" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="C19" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="D19" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="E19" s="8"/>
+      <c r="F19" s="8"/>
+      <c r="G19" s="8"/>
+      <c r="H19" s="8"/>
+      <c r="I19" s="8"/>
+      <c r="J19" s="8"/>
+      <c r="K19" s="8"/>
+    </row>
+    <row r="20" spans="1:11" ht="127.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="7">
+        <v>18</v>
+      </c>
+      <c r="B20" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C20" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="D20" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="E20" s="8"/>
+      <c r="F20" s="8"/>
+      <c r="G20" s="8"/>
+      <c r="H20" s="8"/>
+      <c r="I20" s="8"/>
+      <c r="J20" s="8"/>
+      <c r="K20" s="8"/>
+    </row>
+    <row r="21" spans="1:11" ht="222" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="7">
+        <v>19</v>
+      </c>
+      <c r="B21" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C21" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="D21" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="E21" s="8"/>
+      <c r="F21" s="8"/>
+      <c r="G21" s="8"/>
+      <c r="H21" s="8"/>
+      <c r="I21" s="8"/>
+      <c r="J21" s="8"/>
+      <c r="K21" s="8"/>
+    </row>
+    <row r="22" spans="1:11" ht="222" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="7">
+        <v>20</v>
+      </c>
+      <c r="B22" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C22" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="D22" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="E22" s="8"/>
+      <c r="F22" s="8"/>
+      <c r="G22" s="8"/>
+      <c r="H22" s="8"/>
+      <c r="I22" s="8"/>
+      <c r="J22" s="8"/>
+      <c r="K22" s="8"/>
+    </row>
+    <row r="23" spans="1:11" ht="96" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="7">
+        <v>21</v>
+      </c>
+      <c r="B23" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C23" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="D23" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="E23" s="8"/>
+      <c r="F23" s="8"/>
+      <c r="G23" s="8"/>
+      <c r="H23" s="8"/>
+      <c r="I23" s="8"/>
+      <c r="J23" s="8"/>
+      <c r="K23" s="8"/>
+    </row>
+    <row r="24" spans="1:11" ht="80.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="7">
+        <v>22</v>
+      </c>
+      <c r="B24" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C24" s="8" t="s">
+        <v>97</v>
+      </c>
+      <c r="D24" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="E24" s="8"/>
+      <c r="F24" s="8"/>
+      <c r="G24" s="8"/>
+      <c r="H24" s="8"/>
+      <c r="I24" s="8"/>
+      <c r="J24" s="8"/>
+      <c r="K24" s="8"/>
+    </row>
+    <row r="25" spans="1:11" ht="96" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="7">
+        <v>23</v>
+      </c>
+      <c r="B25" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C25" s="8" t="s">
+        <v>99</v>
+      </c>
+      <c r="D25" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="E25" s="8"/>
+      <c r="F25" s="8"/>
+      <c r="G25" s="8"/>
+      <c r="H25" s="8"/>
+      <c r="I25" s="8"/>
+      <c r="J25" s="8"/>
+      <c r="K25" s="8"/>
+    </row>
+    <row r="26" spans="1:11" ht="16.5" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="55" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A55" s="6"/>
+      <c r="B55" s="6"/>
+      <c r="C55" s="6"/>
+      <c r="D55" s="6"/>
+      <c r="E55" s="6"/>
+      <c r="F55" s="6"/>
+      <c r="G55" s="6"/>
+      <c r="H55" s="6"/>
+      <c r="I55" s="6"/>
+    </row>
+    <row r="56" spans="1:9" ht="16.5" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:K1"/>
@@ -1530,10 +2082,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A08E240A-CAE5-4B6F-872D-9A32F7494C09}">
-  <dimension ref="A2:K11"/>
+  <dimension ref="A2:K20"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1587,10 +2139,10 @@
         <v>12</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="D3" s="11" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="E3" s="10"/>
       <c r="F3" s="10"/>
@@ -1608,10 +2160,10 @@
         <v>12</v>
       </c>
       <c r="C4" s="13" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="E4" s="13"/>
       <c r="F4" s="13"/>
@@ -1629,10 +2181,10 @@
         <v>12</v>
       </c>
       <c r="C5" s="15" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="E5" s="15"/>
       <c r="F5" s="15"/>
@@ -1650,10 +2202,10 @@
         <v>12</v>
       </c>
       <c r="C6" s="15" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="E6" s="15"/>
       <c r="F6" s="15"/>
@@ -1671,10 +2223,10 @@
         <v>12</v>
       </c>
       <c r="C7" s="15" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="E7" s="15"/>
       <c r="F7" s="15"/>
@@ -1692,10 +2244,10 @@
         <v>12</v>
       </c>
       <c r="C8" s="15" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="E8" s="15"/>
       <c r="F8" s="15"/>
@@ -1713,10 +2265,10 @@
         <v>12</v>
       </c>
       <c r="C9" s="15" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="E9" s="15"/>
       <c r="F9" s="15"/>
@@ -1734,10 +2286,10 @@
         <v>12</v>
       </c>
       <c r="C10" s="15" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="E10" s="15"/>
       <c r="F10" s="15"/>
@@ -1747,18 +2299,201 @@
       <c r="J10" s="15"/>
       <c r="K10" s="15"/>
     </row>
-    <row r="11" spans="1:11" ht="284.25" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="25">
+    <row r="11" spans="1:11" ht="285" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="14">
         <v>9</v>
       </c>
-      <c r="B11" s="25" t="s">
-        <v>65</v>
-      </c>
-      <c r="C11" s="26" t="s">
-        <v>66</v>
-      </c>
-      <c r="D11" s="24" t="s">
-        <v>67</v>
+      <c r="B11" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="C11" s="15" t="s">
+        <v>63</v>
+      </c>
+      <c r="D11" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="E11" s="15"/>
+      <c r="F11" s="15"/>
+      <c r="G11" s="15"/>
+      <c r="H11" s="15"/>
+      <c r="I11" s="15"/>
+      <c r="J11" s="15"/>
+      <c r="K11" s="15"/>
+    </row>
+    <row r="12" spans="1:11" ht="206.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="14">
+        <v>10</v>
+      </c>
+      <c r="B12" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="C12" s="15" t="s">
+        <v>79</v>
+      </c>
+      <c r="D12" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="E12" s="15"/>
+      <c r="F12" s="15"/>
+      <c r="G12" s="15"/>
+      <c r="H12" s="15"/>
+      <c r="I12" s="15"/>
+      <c r="J12" s="15"/>
+      <c r="K12" s="15"/>
+    </row>
+    <row r="13" spans="1:11" ht="174.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="14">
+        <v>11</v>
+      </c>
+      <c r="B13" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="C13" s="15" t="s">
+        <v>81</v>
+      </c>
+      <c r="D13" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="E13" s="15"/>
+      <c r="F13" s="15"/>
+      <c r="G13" s="15"/>
+      <c r="H13" s="15"/>
+      <c r="I13" s="15"/>
+      <c r="J13" s="15"/>
+      <c r="K13" s="15"/>
+    </row>
+    <row r="14" spans="1:11" ht="253.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="14">
+        <v>12</v>
+      </c>
+      <c r="B14" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="C14" s="15" t="s">
+        <v>84</v>
+      </c>
+      <c r="D14" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="E14" s="15"/>
+      <c r="F14" s="15"/>
+      <c r="G14" s="15"/>
+      <c r="H14" s="15"/>
+      <c r="I14" s="15"/>
+      <c r="J14" s="15"/>
+      <c r="K14" s="15"/>
+    </row>
+    <row r="15" spans="1:11" ht="253.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="14">
+        <v>13</v>
+      </c>
+      <c r="B15" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="C15" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="D15" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="E15" s="15"/>
+      <c r="F15" s="15"/>
+      <c r="G15" s="15"/>
+      <c r="H15" s="15"/>
+      <c r="I15" s="15"/>
+      <c r="J15" s="15"/>
+      <c r="K15" s="15"/>
+    </row>
+    <row r="16" spans="1:11" ht="159" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="14">
+        <v>14</v>
+      </c>
+      <c r="B16" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="C16" s="15" t="s">
+        <v>87</v>
+      </c>
+      <c r="D16" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="E16" s="15"/>
+      <c r="F16" s="15"/>
+      <c r="G16" s="15"/>
+      <c r="H16" s="15"/>
+      <c r="I16" s="15"/>
+      <c r="J16" s="15"/>
+      <c r="K16" s="15"/>
+    </row>
+    <row r="17" spans="1:11" ht="143.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="14">
+        <v>15</v>
+      </c>
+      <c r="B17" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="C17" s="15" t="s">
+        <v>88</v>
+      </c>
+      <c r="D17" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="E17" s="15"/>
+      <c r="F17" s="15"/>
+      <c r="G17" s="15"/>
+      <c r="H17" s="15"/>
+      <c r="I17" s="15"/>
+      <c r="J17" s="15"/>
+      <c r="K17" s="15"/>
+    </row>
+    <row r="18" spans="1:11" ht="206.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="14">
+        <v>16</v>
+      </c>
+      <c r="B18" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="C18" s="15" t="s">
+        <v>90</v>
+      </c>
+      <c r="D18" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="E18" s="15"/>
+      <c r="F18" s="15"/>
+      <c r="G18" s="15"/>
+      <c r="H18" s="15"/>
+      <c r="I18" s="15"/>
+      <c r="J18" s="15"/>
+      <c r="K18" s="15"/>
+    </row>
+    <row r="19" spans="1:11" ht="174.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="14">
+        <v>17</v>
+      </c>
+      <c r="B19" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="C19" s="15" t="s">
+        <v>92</v>
+      </c>
+      <c r="D19" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="E19" s="15"/>
+      <c r="F19" s="15"/>
+      <c r="G19" s="15"/>
+      <c r="H19" s="15"/>
+      <c r="I19" s="15"/>
+      <c r="J19" s="15"/>
+      <c r="K19" s="15"/>
+    </row>
+    <row r="20" spans="1:11" ht="32.25" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="25"/>
+      <c r="B20" s="25"/>
+      <c r="C20" s="26"/>
+      <c r="D20" s="24" t="s">
+        <v>75</v>
       </c>
     </row>
   </sheetData>
@@ -1770,8 +2505,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{45C76CEF-C2B4-465C-9D00-2F21483FAE24}">
   <dimension ref="A1:K6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1823,13 +2558,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="17" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C2" s="18" t="s">
-        <v>45</v>
-      </c>
-      <c r="D2" s="16" t="s">
-        <v>46</v>
+        <v>42</v>
+      </c>
+      <c r="D2" s="27" t="s">
+        <v>43</v>
       </c>
       <c r="E2" s="18"/>
       <c r="F2" s="18"/>
@@ -1847,10 +2582,10 @@
         <v>12</v>
       </c>
       <c r="C3" s="18" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="D3" s="16" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="E3" s="20"/>
       <c r="F3" s="20"/>
@@ -1868,10 +2603,10 @@
         <v>12</v>
       </c>
       <c r="C4" s="21" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D4" s="23" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="E4" s="20"/>
       <c r="F4" s="20"/>
@@ -1889,10 +2624,10 @@
         <v>12</v>
       </c>
       <c r="C5" s="21" t="s">
+        <v>48</v>
+      </c>
+      <c r="D5" s="22" t="s">
         <v>51</v>
-      </c>
-      <c r="D5" s="22" t="s">
-        <v>55</v>
       </c>
       <c r="E5" s="20"/>
       <c r="F5" s="20"/>
@@ -1913,7 +2648,7 @@
         <v>25</v>
       </c>
       <c r="D6" s="16" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="E6" s="20"/>
       <c r="F6" s="20"/>

</xml_diff>

<commit_message>
updates few more steps
updates few more steps
</commit_message>
<xml_diff>
--- a/manualSteps/PrePostDeploymentSteps.xlsx
+++ b/manualSteps/PrePostDeploymentSteps.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\css116284\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{8E1E5F34-2F85-40C1-96C2-9ADA9F2D8D4C}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{C407AE5B-3388-4A65-AF23-A8DD66259D04}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="16575" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2402,8 +2402,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A08E240A-CAE5-4B6F-872D-9A32F7494C09}">
   <dimension ref="A2:K38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="A33" sqref="A33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -3049,7 +3049,9 @@
       <c r="K28" s="15"/>
     </row>
     <row r="29" spans="1:11" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="14"/>
+      <c r="A29" s="14">
+        <v>27</v>
+      </c>
       <c r="B29" s="14"/>
       <c r="C29" s="15"/>
       <c r="D29" s="8"/>

</xml_diff>

<commit_message>
Changes made to PrePostDeployment Steps
Changes made to PrePostDeployment Steps
</commit_message>
<xml_diff>
--- a/manualSteps/PrePostDeploymentSteps.xlsx
+++ b/manualSteps/PrePostDeploymentSteps.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\css116284\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\css118461\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{C407AE5B-3388-4A65-AF23-A8DD66259D04}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="16575" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="16575" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="PreDeploymentSteps" sheetId="1" r:id="rId1"/>
@@ -22,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="151">
   <si>
     <t>Steps</t>
   </si>
@@ -645,10 +644,6 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">
-</t>
-  </si>
-  <si>
     <t xml:space="preserve">Goto  Setup 
 QuickFind  Communities 
 Community Settings
@@ -827,9 +822,6 @@
 Click on 'Save' button.</t>
   </si>
   <si>
-    <t>Add "Visualforce" page in "Payment" Site which created in 15th Step.</t>
-  </si>
-  <si>
     <t>Goto -&gt; Setup -&gt; User Interface -&gt; Sites and Domains -&gt; Sites
 Click on "Edit" button under "Site Visualforce Page"
 Add "Visualforce Page" -&gt; nctETMembershipPaymentPage, nctMembershipPayementPage, nctPaymentHubErrorMsgPage, nctPaymentHubPage, nctPaymentHubSuccessMsgPage.
@@ -949,14 +941,6 @@
   </si>
   <si>
     <t xml:space="preserve">MAHANTH </t>
-  </si>
-  <si>
-    <t>Goto -&gt; Setup -&gt; User Interface -&gt; Custom Labels
-Click on "New" button.
-Enter "PAYMENTSTATUSURL" value under "Short Description" field
-Enter "PAYMENTSTATUSURL" value under "Name" field
-Enter "Payment link Site which we did in Step-21" value under "value" field.
-Click on "Save" button.</t>
   </si>
   <si>
     <t>Account Contact Relationship</t>
@@ -1043,11 +1027,172 @@
 Click Save
 </t>
   </si>
+  <si>
+    <t>Create "Payment Link URL" custom label.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Create Custom Label "Payment Link URL" Goto -&gt; Setup -&gt; Build -&gt;Create -&gt; Custom Labels
+Click New
+Fill the following fields with below values.
+  1. Short Description : Payment Link URL
+  2. Name : Payment_Link_URL
+  3. Value : "PaymentLink -Site Url"?paymentId=
+    Ex: -https://preuat-mynct.cs102.force.com/PaymentLinkProcessor?paymentId=
+Click Save.
+</t>
+  </si>
+  <si>
+    <t>Create "PAYMENT_SITE_URL" custom label.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Create Custom Label "PAYMENT_SITE_URL" Goto -&gt; Setup -&gt; Build -&gt;Create -&gt; Custom Labels
+Click New
+Fill the following fields with below values.
+  1. Short Description : PAYMENT_SITE_URL
+  2. Name : PAYMENT_SITE_URL
+  3. Value : "Payment -Site Url"
+    Ex: -https://testdeploy-mynct.cs100.force.com/nctMembershipPaymentPage
+Click Save.
+</t>
+  </si>
+  <si>
+    <t>Create "SF_INSTANCE" custom label.</t>
+  </si>
+  <si>
+    <t>Create "API_TOKEN" custom label.</t>
+  </si>
+  <si>
+    <t>Create "ENDPOINTOAUTH" custom label.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Create Custom Label "SF_INSTANCE" Goto -&gt; Setup -&gt; Build -&gt;Create -&gt; Custom Labels
+Click New
+Fill the following fields with below values.
+  1. Short Description : SF_INSTANCE
+  2. Name : SF_INSTANCE
+  3. Value : "Salesforce Instance Url"
+    Ex: -https://cs108.salesforce.com
+Click Save.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Create Custom Label "ENDPOINTOAUTH" Goto -&gt; Setup -&gt; Build -&gt;Create -&gt; Custom Labels
+Click New
+Fill the following fields with below values.
+  1. Short Description : ENDPOINTOAUTH
+  2. Name : ENDPOINTOAUTH
+  3. Value : https://test.salesforce.com/services/oauth2/token?
+    Ex: -https://test.salesforce.com/services/oauth2/token?
+Click Save.
+</t>
+  </si>
+  <si>
+    <t>Create "CLIENTID" custom label.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Create Custom Label "CLIENTID" Goto -&gt; Setup -&gt; Build -&gt;Create -&gt; Custom Labels
+Click New
+Fill the following fields with below values.
+  1. Short Description : CLIENTID
+  2. Name : CLIENTID
+  3. Value : "PAYMENT-HUB : Client Id"
+    Ex: -3MVG9llQY5kM9T6dLJQdcZnV9pOGDMM6ONAFoTiZ5jTG34DQvBCb3nGe5YogBoZ8NLt8i.NfOUDmEt00uvRsm
+Click Save.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Create Custom Label "API_TOKEN" Goto -&gt; Setup -&gt; Build -&gt;Create -&gt; Custom Labels
+Click New
+Fill the following fields with below values.
+  1. Short Description : API_TOKEN
+  2. Name : API_TOKEN
+  3. Value : "PAYMENT-HUB: API TOKEN"
+    Ex:-qJKBsZNzdqClIuKvGx0zIApojFpYSIBSFwDA2qalvq2BljHVIU1ktRM5KHfNciQyW9PRK4bxYgiNwxKuqokMK7zjfzcM47cj53crArfpl8siZD9vpm9u4swxg3nl75sD32BzZimaSvGnAsIBbQmwneacYkt9wSpddoxgJRJQo43esYuWTxp8SHzE8jgBv50Itvtu68wk
+Click Save.
+</t>
+  </si>
+  <si>
+    <t>Create "CLIENT_SECRET" custom label.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Create Custom Label "CLIENT_SECRET" Goto -&gt; Setup -&gt; Build -&gt;Create -&gt; Custom Labels
+Click New
+Fill the following fields with below values.
+  1. Short Description : CLIENT_SECRET
+  2. Name : CLIENT_SECRET
+  3. Value : "PAYMENT-HUB: CLIENT_SECRET"
+    Ex: -FE86B45521682BF5B801A881D6E75AC84A6009D37D0D4C47B51E25CCB51CA0A7
+Click Save.
+</t>
+  </si>
+  <si>
+    <t>Create "ENDPOINT_USERNAME" custom label.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Create Custom Label "ENDPOINT_USERNAME" Goto -&gt; Setup -&gt; Build -&gt;Create -&gt; Custom Labels
+Click New
+Fill the following fields with below values.
+  1. Short Description : ENDPOINT_USERNAME
+  2. Name : ENDPOINT_USERNAME
+  3. Value : "PAYMENT-HUB: ENDPOINT_USERNAME"
+    Ex: -payment.api@nct.org.uk.testdeploy
+Click Save.
+</t>
+  </si>
+  <si>
+    <t>Create "ENDPOINT_PASSWORD" custom label.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Create Custom Label "ENDPOINT_PASSWORD" Goto -&gt; Setup -&gt; Build -&gt;Create -&gt; Custom Labels
+Click New
+Fill the following fields with below values.
+  1. Short Description : ENDPOINT_PASSWORD
+  2. Name : ENDPOINT_PASSWORD
+  3. Value : "PAYMENT-HUB: ENDPOINT_PASSWORD"
+    Ex: -api@nct@123lWwQJknCS3Z9GmdRxX1OebUkN
+Click Save.
+</t>
+  </si>
+  <si>
+    <t>Add "Visualforce" page in "Payment" Site which created in 36th Step.</t>
+  </si>
+  <si>
+    <t>Goto -&gt; Setup -&gt; User Interface -&gt; Custom Labels
+Click on "New" button.
+Enter "PAYMENTSTATUSURL" value under "Short Description" field
+Enter "PAYMENTSTATUSURL" value under "Name" field
+Enter "Payment link Site which we did in Step-36" value under "value" field.
+Click on "Save" button.</t>
+  </si>
+  <si>
+    <t>Add "Sandbox" url in Remote Site Settings.</t>
+  </si>
+  <si>
+    <t>Goto -&gt; Setup -&gt; Settings -&gt; Remote Site Settings
+Click on "New Remote Site" button.
+Fill the following fields with below values.
+  1. Remote Site Name : Sandbox
+  2. Remote Site URL : https://test.salesforce.com
+    Ex: -https://test.salesforce.com
+Click Save.</t>
+  </si>
+  <si>
+    <t>Add "SandboxInstance" url in Remote Site Settings.</t>
+  </si>
+  <si>
+    <t>Goto -&gt; Setup -&gt; Settings -&gt; Remote Site Settings
+Click on "New Remote Site" button.
+Fill the following fields with below values.
+  1. Remote Site Name : SandboxInstance
+  2. Remote Site URL : https://cs100.salesforce.com -&gt; Instance
+    Ex: -https://cs100.salesforce.com
+Click Save.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -1124,7 +1269,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1134,6 +1279,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1209,7 +1360,7 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1280,12 +1431,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="13" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -1293,16 +1438,23 @@
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -1322,7 +1474,7 @@
     <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="13" xr:uid="{00000000-0005-0000-0000-00003B000000}"/>
+    <cellStyle name="Normal 2" xfId="13"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
@@ -1707,11 +1859,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L58"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+    <sheetView topLeftCell="A13" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1726,17 +1878,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A1" s="32"/>
-      <c r="B1" s="32"/>
-      <c r="C1" s="32"/>
-      <c r="D1" s="32"/>
-      <c r="E1" s="32"/>
-      <c r="F1" s="32"/>
-      <c r="G1" s="32"/>
-      <c r="H1" s="32"/>
-      <c r="I1" s="32"/>
-      <c r="J1" s="32"/>
-      <c r="K1" s="32"/>
+      <c r="A1" s="33"/>
+      <c r="B1" s="33"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="33"/>
+      <c r="G1" s="33"/>
+      <c r="H1" s="33"/>
+      <c r="I1" s="33"/>
+      <c r="J1" s="33"/>
+      <c r="K1" s="33"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -1784,13 +1936,13 @@
         <v>11</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="D3" s="6" t="s">
         <v>23</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="F3" s="6"/>
       <c r="G3" s="6"/>
@@ -1813,7 +1965,7 @@
         <v>18</v>
       </c>
       <c r="E4" s="8" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="F4" s="8"/>
       <c r="G4" s="8"/>
@@ -1836,7 +1988,7 @@
         <v>22</v>
       </c>
       <c r="E5" s="8" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="F5" s="8"/>
       <c r="G5" s="8"/>
@@ -1859,7 +2011,7 @@
         <v>21</v>
       </c>
       <c r="E6" s="8" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="F6" s="8"/>
       <c r="G6" s="8"/>
@@ -1882,7 +2034,7 @@
         <v>25</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="F7" s="8"/>
       <c r="G7" s="8"/>
@@ -1905,7 +2057,7 @@
         <v>20</v>
       </c>
       <c r="E8" s="8" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="F8" s="8"/>
       <c r="G8" s="8"/>
@@ -1928,7 +2080,7 @@
         <v>19</v>
       </c>
       <c r="E9" s="8" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="F9" s="8"/>
       <c r="G9" s="8"/>
@@ -1951,7 +2103,7 @@
         <v>31</v>
       </c>
       <c r="E10" s="8" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="F10" s="8"/>
       <c r="G10" s="8"/>
@@ -1974,7 +2126,7 @@
         <v>32</v>
       </c>
       <c r="E11" s="8" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="F11" s="8"/>
       <c r="G11" s="8"/>
@@ -1997,7 +2149,7 @@
         <v>73</v>
       </c>
       <c r="E12" s="8" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="F12" s="8"/>
       <c r="G12" s="8"/>
@@ -2020,7 +2172,7 @@
         <v>72</v>
       </c>
       <c r="E13" s="8" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="F13" s="8"/>
       <c r="G13" s="8"/>
@@ -2043,7 +2195,7 @@
         <v>71</v>
       </c>
       <c r="E14" s="8" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="F14" s="8"/>
       <c r="G14" s="8"/>
@@ -2066,7 +2218,7 @@
         <v>70</v>
       </c>
       <c r="E15" s="8" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="F15" s="8"/>
       <c r="G15" s="8"/>
@@ -2089,7 +2241,7 @@
         <v>69</v>
       </c>
       <c r="E16" s="8" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="F16" s="8"/>
       <c r="G16" s="8"/>
@@ -2112,7 +2264,7 @@
         <v>68</v>
       </c>
       <c r="E17" s="8" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="F17" s="8"/>
       <c r="G17" s="8"/>
@@ -2135,7 +2287,7 @@
         <v>67</v>
       </c>
       <c r="E18" s="8" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="F18" s="8"/>
       <c r="G18" s="8"/>
@@ -2158,7 +2310,7 @@
         <v>66</v>
       </c>
       <c r="E19" s="8" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="F19" s="8"/>
       <c r="G19" s="8"/>
@@ -2178,10 +2330,10 @@
         <v>15</v>
       </c>
       <c r="D20" s="8" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E20" s="8" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="F20" s="8"/>
       <c r="G20" s="8"/>
@@ -2198,13 +2350,13 @@
         <v>11</v>
       </c>
       <c r="C21" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="D21" s="8" t="s">
         <v>76</v>
       </c>
-      <c r="D21" s="8" t="s">
-        <v>77</v>
-      </c>
       <c r="E21" s="8" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="F21" s="8"/>
       <c r="G21" s="8"/>
@@ -2221,13 +2373,13 @@
         <v>11</v>
       </c>
       <c r="C22" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="D22" s="8" t="s">
         <v>76</v>
       </c>
-      <c r="D22" s="8" t="s">
-        <v>77</v>
-      </c>
       <c r="E22" s="8" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="F22" s="8"/>
       <c r="G22" s="8"/>
@@ -2236,22 +2388,12 @@
       <c r="J22" s="8"/>
       <c r="K22" s="8"/>
     </row>
-    <row r="23" spans="1:11" ht="96" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="7">
-        <v>21</v>
-      </c>
-      <c r="B23" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="C23" s="8" t="s">
-        <v>94</v>
-      </c>
-      <c r="D23" s="8" t="s">
-        <v>95</v>
-      </c>
-      <c r="E23" s="8" t="s">
-        <v>116</v>
-      </c>
+    <row r="23" spans="1:11" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="7"/>
+      <c r="B23" s="8"/>
+      <c r="C23" s="8"/>
+      <c r="D23" s="8"/>
+      <c r="E23" s="8"/>
       <c r="F23" s="8"/>
       <c r="G23" s="8"/>
       <c r="H23" s="8"/>
@@ -2259,22 +2401,12 @@
       <c r="J23" s="8"/>
       <c r="K23" s="8"/>
     </row>
-    <row r="24" spans="1:11" ht="80.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="7">
-        <v>22</v>
-      </c>
-      <c r="B24" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="C24" s="8" t="s">
-        <v>96</v>
-      </c>
-      <c r="D24" s="8" t="s">
-        <v>97</v>
-      </c>
-      <c r="E24" s="8" t="s">
-        <v>116</v>
-      </c>
+    <row r="24" spans="1:11" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="7"/>
+      <c r="B24" s="8"/>
+      <c r="C24" s="8"/>
+      <c r="D24" s="8"/>
+      <c r="E24" s="8"/>
       <c r="F24" s="8"/>
       <c r="G24" s="8"/>
       <c r="H24" s="8"/>
@@ -2282,22 +2414,12 @@
       <c r="J24" s="8"/>
       <c r="K24" s="8"/>
     </row>
-    <row r="25" spans="1:11" ht="96" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="7">
-        <v>23</v>
-      </c>
-      <c r="B25" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="C25" s="8" t="s">
-        <v>98</v>
-      </c>
-      <c r="D25" s="8" t="s">
-        <v>122</v>
-      </c>
-      <c r="E25" s="8" t="s">
-        <v>116</v>
-      </c>
+    <row r="25" spans="1:11" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="7"/>
+      <c r="B25" s="8"/>
+      <c r="C25" s="8"/>
+      <c r="D25" s="8"/>
+      <c r="E25" s="8"/>
       <c r="F25" s="8"/>
       <c r="G25" s="8"/>
       <c r="H25" s="8"/>
@@ -2399,11 +2521,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A08E240A-CAE5-4B6F-872D-9A32F7494C09}">
-  <dimension ref="A2:K38"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:K43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="A33" sqref="A33"/>
+    <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
+      <selection activeCell="C42" sqref="C42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2464,7 +2586,7 @@
         <v>54</v>
       </c>
       <c r="E3" s="10" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="F3" s="10"/>
       <c r="G3" s="10"/>
@@ -2487,7 +2609,7 @@
         <v>52</v>
       </c>
       <c r="E4" s="13" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="F4" s="13"/>
       <c r="G4" s="13"/>
@@ -2510,7 +2632,7 @@
         <v>51</v>
       </c>
       <c r="E5" s="15" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="F5" s="15"/>
       <c r="G5" s="15"/>
@@ -2533,7 +2655,7 @@
         <v>53</v>
       </c>
       <c r="E6" s="15" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="F6" s="15"/>
       <c r="G6" s="15"/>
@@ -2556,7 +2678,7 @@
         <v>55</v>
       </c>
       <c r="E7" s="15" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="F7" s="15"/>
       <c r="G7" s="15"/>
@@ -2579,7 +2701,7 @@
         <v>56</v>
       </c>
       <c r="E8" s="15" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="F8" s="15"/>
       <c r="G8" s="15"/>
@@ -2602,7 +2724,7 @@
         <v>57</v>
       </c>
       <c r="E9" s="15" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="F9" s="15"/>
       <c r="G9" s="15"/>
@@ -2625,7 +2747,7 @@
         <v>58</v>
       </c>
       <c r="E10" s="15" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="F10" s="15"/>
       <c r="G10" s="15"/>
@@ -2648,7 +2770,7 @@
         <v>61</v>
       </c>
       <c r="E11" s="15" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="F11" s="15"/>
       <c r="G11" s="15"/>
@@ -2665,13 +2787,13 @@
         <v>60</v>
       </c>
       <c r="C12" s="15" t="s">
+        <v>77</v>
+      </c>
+      <c r="D12" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="D12" s="8" t="s">
-        <v>79</v>
-      </c>
       <c r="E12" s="15" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="F12" s="15"/>
       <c r="G12" s="15"/>
@@ -2688,13 +2810,13 @@
         <v>60</v>
       </c>
       <c r="C13" s="15" t="s">
+        <v>79</v>
+      </c>
+      <c r="D13" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="D13" s="8" t="s">
-        <v>81</v>
-      </c>
       <c r="E13" s="15" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="F13" s="15"/>
       <c r="G13" s="15"/>
@@ -2711,13 +2833,13 @@
         <v>60</v>
       </c>
       <c r="C14" s="15" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D14" s="8" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E14" s="15" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="F14" s="15"/>
       <c r="G14" s="15"/>
@@ -2734,13 +2856,13 @@
         <v>60</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E15" s="15" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="F15" s="15"/>
       <c r="G15" s="15"/>
@@ -2757,13 +2879,13 @@
         <v>60</v>
       </c>
       <c r="C16" s="15" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E16" s="15" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="F16" s="15"/>
       <c r="G16" s="15"/>
@@ -2780,13 +2902,13 @@
         <v>60</v>
       </c>
       <c r="C17" s="15" t="s">
+        <v>86</v>
+      </c>
+      <c r="D17" s="8" t="s">
         <v>87</v>
       </c>
-      <c r="D17" s="8" t="s">
-        <v>88</v>
-      </c>
       <c r="E17" s="15" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="F17" s="15"/>
       <c r="G17" s="15"/>
@@ -2803,13 +2925,13 @@
         <v>60</v>
       </c>
       <c r="C18" s="15" t="s">
+        <v>88</v>
+      </c>
+      <c r="D18" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="D18" s="8" t="s">
-        <v>90</v>
-      </c>
       <c r="E18" s="15" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="F18" s="15"/>
       <c r="G18" s="15"/>
@@ -2826,13 +2948,13 @@
         <v>60</v>
       </c>
       <c r="C19" s="15" t="s">
+        <v>90</v>
+      </c>
+      <c r="D19" s="8" t="s">
         <v>91</v>
       </c>
-      <c r="D19" s="8" t="s">
-        <v>92</v>
-      </c>
       <c r="E19" s="15" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="F19" s="15"/>
       <c r="G19" s="15"/>
@@ -2849,13 +2971,13 @@
         <v>60</v>
       </c>
       <c r="C20" s="15" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="D20" s="8" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="E20" s="15" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="F20" s="15"/>
       <c r="G20" s="15"/>
@@ -2872,13 +2994,13 @@
         <v>60</v>
       </c>
       <c r="C21" s="15" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="D21" s="8" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="E21" s="15" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="F21" s="15"/>
       <c r="G21" s="15"/>
@@ -2892,16 +3014,16 @@
         <v>20</v>
       </c>
       <c r="B22" s="15" t="s">
-        <v>107</v>
-      </c>
-      <c r="C22" s="31" t="s">
-        <v>106</v>
+        <v>105</v>
+      </c>
+      <c r="C22" s="27" t="s">
+        <v>104</v>
       </c>
       <c r="D22" s="8" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="E22" s="15" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="F22" s="15"/>
       <c r="G22" s="15"/>
@@ -2918,13 +3040,13 @@
         <v>11</v>
       </c>
       <c r="C23" s="15" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D23" s="8" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="E23" s="15" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="F23" s="15"/>
       <c r="G23" s="15"/>
@@ -2933,51 +3055,51 @@
       <c r="J23" s="15"/>
       <c r="K23" s="15"/>
     </row>
-    <row r="24" spans="1:11" ht="222" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="14">
+    <row r="24" spans="1:11" s="31" customFormat="1" ht="222" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="28">
         <v>22</v>
       </c>
-      <c r="B24" s="14" t="s">
-        <v>110</v>
-      </c>
-      <c r="C24" s="15" t="s">
-        <v>109</v>
-      </c>
-      <c r="D24" s="8" t="s">
+      <c r="B24" s="28" t="s">
         <v>108</v>
       </c>
-      <c r="E24" s="15" t="s">
-        <v>113</v>
-      </c>
-      <c r="F24" s="15"/>
-      <c r="G24" s="15"/>
-      <c r="H24" s="15"/>
-      <c r="I24" s="15"/>
-      <c r="J24" s="15"/>
-      <c r="K24" s="15"/>
-    </row>
-    <row r="25" spans="1:11" ht="159" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="14">
+      <c r="C24" s="29" t="s">
+        <v>107</v>
+      </c>
+      <c r="D24" s="30" t="s">
+        <v>106</v>
+      </c>
+      <c r="E24" s="29" t="s">
+        <v>111</v>
+      </c>
+      <c r="F24" s="29"/>
+      <c r="G24" s="29"/>
+      <c r="H24" s="29"/>
+      <c r="I24" s="29"/>
+      <c r="J24" s="29"/>
+      <c r="K24" s="29"/>
+    </row>
+    <row r="25" spans="1:11" s="31" customFormat="1" ht="159" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="28">
         <v>23</v>
       </c>
-      <c r="B25" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="C25" s="15" t="s">
-        <v>117</v>
-      </c>
-      <c r="D25" s="8" t="s">
-        <v>125</v>
-      </c>
-      <c r="E25" s="15" t="s">
-        <v>113</v>
-      </c>
-      <c r="F25" s="15"/>
-      <c r="G25" s="15"/>
-      <c r="H25" s="15"/>
-      <c r="I25" s="15"/>
-      <c r="J25" s="15"/>
-      <c r="K25" s="15"/>
+      <c r="B25" s="28" t="s">
+        <v>11</v>
+      </c>
+      <c r="C25" s="29" t="s">
+        <v>115</v>
+      </c>
+      <c r="D25" s="30" t="s">
+        <v>122</v>
+      </c>
+      <c r="E25" s="29" t="s">
+        <v>111</v>
+      </c>
+      <c r="F25" s="29"/>
+      <c r="G25" s="29"/>
+      <c r="H25" s="29"/>
+      <c r="I25" s="29"/>
+      <c r="J25" s="29"/>
+      <c r="K25" s="29"/>
     </row>
     <row r="26" spans="1:11" ht="127.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="14">
@@ -2987,13 +3109,13 @@
         <v>11</v>
       </c>
       <c r="C26" s="15" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="D26" s="8" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="E26" s="15" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="F26" s="15"/>
       <c r="G26" s="15"/>
@@ -3010,13 +3132,13 @@
         <v>60</v>
       </c>
       <c r="C27" s="15" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="D27" s="8" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="E27" s="15" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="F27" s="15"/>
       <c r="G27" s="15"/>
@@ -3033,13 +3155,13 @@
         <v>60</v>
       </c>
       <c r="C28" s="8" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="D28" s="8" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="E28" s="15" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="F28" s="15"/>
       <c r="G28" s="15"/>
@@ -3048,14 +3170,22 @@
       <c r="J28" s="15"/>
       <c r="K28" s="15"/>
     </row>
-    <row r="29" spans="1:11" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:11" ht="143.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="14">
         <v>27</v>
       </c>
-      <c r="B29" s="14"/>
-      <c r="C29" s="15"/>
-      <c r="D29" s="8"/>
-      <c r="E29" s="15"/>
+      <c r="B29" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="C29" s="15" t="s">
+        <v>127</v>
+      </c>
+      <c r="D29" s="8" t="s">
+        <v>128</v>
+      </c>
+      <c r="E29" s="15" t="s">
+        <v>114</v>
+      </c>
       <c r="F29" s="15"/>
       <c r="G29" s="15"/>
       <c r="H29" s="15"/>
@@ -3063,12 +3193,22 @@
       <c r="J29" s="15"/>
       <c r="K29" s="15"/>
     </row>
-    <row r="30" spans="1:11" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="14"/>
-      <c r="B30" s="14"/>
-      <c r="C30" s="15"/>
-      <c r="D30" s="8"/>
-      <c r="E30" s="15"/>
+    <row r="30" spans="1:11" ht="143.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="14">
+        <v>28</v>
+      </c>
+      <c r="B30" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="C30" s="15" t="s">
+        <v>129</v>
+      </c>
+      <c r="D30" s="8" t="s">
+        <v>130</v>
+      </c>
+      <c r="E30" s="15" t="s">
+        <v>114</v>
+      </c>
       <c r="F30" s="15"/>
       <c r="G30" s="15"/>
       <c r="H30" s="15"/>
@@ -3076,12 +3216,22 @@
       <c r="J30" s="15"/>
       <c r="K30" s="15"/>
     </row>
-    <row r="31" spans="1:11" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="14"/>
-      <c r="B31" s="14"/>
-      <c r="C31" s="15"/>
-      <c r="D31" s="8"/>
-      <c r="E31" s="15"/>
+    <row r="31" spans="1:11" ht="143.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="14">
+        <v>29</v>
+      </c>
+      <c r="B31" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="C31" s="15" t="s">
+        <v>131</v>
+      </c>
+      <c r="D31" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="E31" s="15" t="s">
+        <v>114</v>
+      </c>
       <c r="F31" s="15"/>
       <c r="G31" s="15"/>
       <c r="H31" s="15"/>
@@ -3089,12 +3239,22 @@
       <c r="J31" s="15"/>
       <c r="K31" s="15"/>
     </row>
-    <row r="32" spans="1:11" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="14"/>
-      <c r="B32" s="14"/>
-      <c r="C32" s="15"/>
-      <c r="D32" s="8"/>
-      <c r="E32" s="15"/>
+    <row r="32" spans="1:11" ht="190.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="14">
+        <v>30</v>
+      </c>
+      <c r="B32" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="C32" s="15" t="s">
+        <v>132</v>
+      </c>
+      <c r="D32" s="8" t="s">
+        <v>138</v>
+      </c>
+      <c r="E32" s="15" t="s">
+        <v>114</v>
+      </c>
       <c r="F32" s="15"/>
       <c r="G32" s="15"/>
       <c r="H32" s="15"/>
@@ -3102,12 +3262,22 @@
       <c r="J32" s="15"/>
       <c r="K32" s="15"/>
     </row>
-    <row r="33" spans="1:11" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="14"/>
-      <c r="B33" s="14"/>
-      <c r="C33" s="15"/>
-      <c r="D33" s="8"/>
-      <c r="E33" s="15"/>
+    <row r="33" spans="1:11" ht="143.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="14">
+        <v>31</v>
+      </c>
+      <c r="B33" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="C33" s="15" t="s">
+        <v>133</v>
+      </c>
+      <c r="D33" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="E33" s="15" t="s">
+        <v>114</v>
+      </c>
       <c r="F33" s="15"/>
       <c r="G33" s="15"/>
       <c r="H33" s="15"/>
@@ -3115,12 +3285,22 @@
       <c r="J33" s="15"/>
       <c r="K33" s="15"/>
     </row>
-    <row r="34" spans="1:11" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="14"/>
-      <c r="B34" s="14"/>
-      <c r="C34" s="15"/>
-      <c r="D34" s="8"/>
-      <c r="E34" s="15"/>
+    <row r="34" spans="1:11" ht="174.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="14">
+        <v>32</v>
+      </c>
+      <c r="B34" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="C34" s="15" t="s">
+        <v>136</v>
+      </c>
+      <c r="D34" s="8" t="s">
+        <v>137</v>
+      </c>
+      <c r="E34" s="15" t="s">
+        <v>114</v>
+      </c>
       <c r="F34" s="15"/>
       <c r="G34" s="15"/>
       <c r="H34" s="15"/>
@@ -3128,63 +3308,171 @@
       <c r="J34" s="15"/>
       <c r="K34" s="15"/>
     </row>
-    <row r="35" spans="1:11" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="29"/>
-      <c r="B35" s="29"/>
-      <c r="C35" s="30"/>
-      <c r="D35" s="28"/>
-      <c r="E35" s="30"/>
-      <c r="F35" s="30"/>
-      <c r="G35" s="30"/>
-      <c r="H35" s="30"/>
-      <c r="I35" s="30"/>
-      <c r="J35" s="30"/>
-      <c r="K35" s="30"/>
-    </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A36" s="29"/>
-      <c r="B36" s="29"/>
-      <c r="C36" s="30"/>
-      <c r="D36" s="28"/>
-      <c r="E36" s="30"/>
-      <c r="F36" s="30"/>
-      <c r="G36" s="30"/>
-      <c r="H36" s="30"/>
-      <c r="I36" s="30"/>
-      <c r="J36" s="30"/>
-      <c r="K36" s="30"/>
-    </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A37" s="29"/>
-      <c r="B37" s="29"/>
-      <c r="C37" s="30"/>
-      <c r="D37" s="28"/>
-      <c r="E37" s="30"/>
-      <c r="F37" s="30"/>
-      <c r="G37" s="30"/>
-      <c r="H37" s="30"/>
-      <c r="I37" s="30"/>
-      <c r="J37" s="30"/>
-      <c r="K37" s="30"/>
-    </row>
-    <row r="38" spans="1:11" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A38" s="25"/>
-      <c r="B38" s="25"/>
-      <c r="C38" s="26"/>
-      <c r="D38" s="24" t="s">
-        <v>74</v>
-      </c>
-    </row>
+    <row r="35" spans="1:11" ht="143.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="14">
+        <v>33</v>
+      </c>
+      <c r="B35" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="C35" s="15" t="s">
+        <v>139</v>
+      </c>
+      <c r="D35" s="8" t="s">
+        <v>140</v>
+      </c>
+      <c r="E35" s="15" t="s">
+        <v>114</v>
+      </c>
+      <c r="F35" s="26"/>
+      <c r="G35" s="26"/>
+      <c r="H35" s="26"/>
+      <c r="I35" s="26"/>
+      <c r="J35" s="26"/>
+      <c r="K35" s="26"/>
+    </row>
+    <row r="36" spans="1:11" ht="159" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="14">
+        <v>34</v>
+      </c>
+      <c r="B36" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="C36" s="15" t="s">
+        <v>141</v>
+      </c>
+      <c r="D36" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="E36" s="15" t="s">
+        <v>114</v>
+      </c>
+      <c r="F36" s="26"/>
+      <c r="G36" s="26"/>
+      <c r="H36" s="26"/>
+      <c r="I36" s="26"/>
+      <c r="J36" s="26"/>
+      <c r="K36" s="26"/>
+    </row>
+    <row r="37" spans="1:11" ht="159" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="14">
+        <v>35</v>
+      </c>
+      <c r="B37" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="C37" s="15" t="s">
+        <v>143</v>
+      </c>
+      <c r="D37" s="8" t="s">
+        <v>144</v>
+      </c>
+      <c r="E37" s="15" t="s">
+        <v>114</v>
+      </c>
+      <c r="F37" s="26"/>
+      <c r="G37" s="26"/>
+      <c r="H37" s="26"/>
+      <c r="I37" s="26"/>
+      <c r="J37" s="26"/>
+      <c r="K37" s="26"/>
+    </row>
+    <row r="38" spans="1:11" ht="96" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="7">
+        <v>36</v>
+      </c>
+      <c r="B38" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C38" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="D38" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="E38" s="8" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" ht="80.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="7">
+        <v>37</v>
+      </c>
+      <c r="B39" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C39" s="8" t="s">
+        <v>145</v>
+      </c>
+      <c r="D39" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="E39" s="8" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" ht="96" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="7">
+        <v>38</v>
+      </c>
+      <c r="B40" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C40" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="D40" s="8" t="s">
+        <v>146</v>
+      </c>
+      <c r="E40" s="8" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" ht="127.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="32">
+        <v>39</v>
+      </c>
+      <c r="B41" s="32" t="s">
+        <v>60</v>
+      </c>
+      <c r="C41" s="24" t="s">
+        <v>147</v>
+      </c>
+      <c r="D41" s="8" t="s">
+        <v>148</v>
+      </c>
+      <c r="E41" s="24" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" ht="127.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="32">
+        <v>40</v>
+      </c>
+      <c r="B42" s="32" t="s">
+        <v>60</v>
+      </c>
+      <c r="C42" s="24" t="s">
+        <v>149</v>
+      </c>
+      <c r="D42" s="8" t="s">
+        <v>150</v>
+      </c>
+      <c r="E42" s="24" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" ht="16.5" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{45C76CEF-C2B4-465C-9D00-2F21483FAE24}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A8" workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
@@ -3242,7 +3530,7 @@
       <c r="C2" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="D2" s="27" t="s">
+      <c r="D2" s="25" t="s">
         <v>42</v>
       </c>
       <c r="E2" s="18"/>

</xml_diff>

<commit_message>
Post Deployment Step added for Email Opt In
Please verify the changes. Thanks.
</commit_message>
<xml_diff>
--- a/manualSteps/PrePostDeploymentSteps.xlsx
+++ b/manualSteps/PrePostDeploymentSteps.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="16925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\css116318\Documents\GitHub\NCT\nctRepository\Salesforce\manualSteps\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\css116762\Documents\GitHub\Salesforce\manualSteps\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F206BE24-8DED-48EA-9570-5972025CDC30}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="16575" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="16575" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PreDeploymentSteps" sheetId="1" r:id="rId1"/>
@@ -21,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="306" uniqueCount="163">
   <si>
     <t>Steps</t>
   </si>
@@ -1245,11 +1246,25 @@
 Remove Migration reference section
 click save</t>
   </si>
+  <si>
+    <t xml:space="preserve">Go to setup
+Quick find “Tabs”
+Under “Build section” Go to “Rename Tabs &amp; Labels”
+Edit Next to Contacts Tab Name.
+Click on "Next" button.
+Goto "Do Not Call" and edit to "Make A Call".
+Goto "Email Opt Out" and edit "Email Opt In"
+Click save.
+</t>
+  </si>
+  <si>
+    <t>Rename Label Name for Tabs : "Contact”</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -1426,7 +1441,7 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1533,6 +1548,24 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="14">
@@ -1549,7 +1582,7 @@
     <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="13"/>
+    <cellStyle name="Normal 2" xfId="13" xr:uid="{00000000-0005-0000-0000-00000D000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
@@ -1934,11 +1967,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L59"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+    <sheetView topLeftCell="B23" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1953,17 +1986,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A1" s="35"/>
-      <c r="B1" s="35"/>
-      <c r="C1" s="35"/>
-      <c r="D1" s="35"/>
-      <c r="E1" s="35"/>
-      <c r="F1" s="35"/>
-      <c r="G1" s="35"/>
-      <c r="H1" s="35"/>
-      <c r="I1" s="35"/>
-      <c r="J1" s="35"/>
-      <c r="K1" s="35"/>
+      <c r="A1" s="37"/>
+      <c r="B1" s="37"/>
+      <c r="C1" s="37"/>
+      <c r="D1" s="37"/>
+      <c r="E1" s="37"/>
+      <c r="F1" s="37"/>
+      <c r="G1" s="37"/>
+      <c r="H1" s="37"/>
+      <c r="I1" s="37"/>
+      <c r="J1" s="37"/>
+      <c r="K1" s="37"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -2615,11 +2648,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:K43"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A2:K45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B42" workbookViewId="0">
-      <selection activeCell="D47" sqref="D47"/>
+    <sheetView tabSelected="1" topLeftCell="B43" workbookViewId="0">
+      <selection activeCell="C43" sqref="C43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -3529,16 +3562,16 @@
       <c r="A41" s="28">
         <v>39</v>
       </c>
-      <c r="B41" s="28" t="s">
+      <c r="B41" s="41" t="s">
         <v>60</v>
       </c>
-      <c r="C41" s="24" t="s">
+      <c r="C41" s="42" t="s">
         <v>146</v>
       </c>
       <c r="D41" s="8" t="s">
         <v>147</v>
       </c>
-      <c r="E41" s="24" t="s">
+      <c r="E41" s="42" t="s">
         <v>113</v>
       </c>
     </row>
@@ -3546,20 +3579,20 @@
       <c r="A42" s="28">
         <v>40</v>
       </c>
-      <c r="B42" s="28" t="s">
+      <c r="B42" s="39" t="s">
         <v>60</v>
       </c>
-      <c r="C42" s="24" t="s">
+      <c r="C42" s="40" t="s">
         <v>148</v>
       </c>
-      <c r="D42" s="8" t="s">
+      <c r="D42" s="6" t="s">
         <v>149</v>
       </c>
-      <c r="E42" s="24" t="s">
+      <c r="E42" s="40" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="43" spans="1:11" ht="95.25" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:11" ht="96" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="28">
         <v>41</v>
       </c>
@@ -3575,6 +3608,26 @@
       <c r="E43" s="24" t="s">
         <v>110</v>
       </c>
+    </row>
+    <row r="44" spans="1:11" ht="143.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B44" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="C44" s="15" t="s">
+        <v>162</v>
+      </c>
+      <c r="D44" s="8" t="s">
+        <v>161</v>
+      </c>
+      <c r="E44" s="15" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="B45" s="38"/>
+      <c r="C45" s="26"/>
+      <c r="D45" s="35"/>
+      <c r="E45" s="26"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3582,7 +3635,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:K6"/>
   <sheetViews>
     <sheetView topLeftCell="A8" workbookViewId="0">

</xml_diff>